<commit_message>
tested with more headers
</commit_message>
<xml_diff>
--- a/test-headers.xlsx
+++ b/test-headers.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Table 1</t>
   </si>
@@ -29,22 +29,64 @@
     <t>Saint Lauren</t>
   </si>
   <si>
-    <t>Testlink</t>
-  </si>
-  <si>
-    <t>Lorem Ipsum</t>
+    <t>Sain Lauren Link</t>
+  </si>
+  <si>
+    <t>Some copy about Saint Lauren</t>
   </si>
   <si>
     <t>Burberry</t>
   </si>
   <si>
+    <t>Burberry Link</t>
+  </si>
+  <si>
+    <t>Some copy about Burberry</t>
+  </si>
+  <si>
     <t>Channel</t>
   </si>
   <si>
+    <t>Channel Link</t>
+  </si>
+  <si>
+    <t>Some copy about Channel</t>
+  </si>
+  <si>
     <t>Louis V</t>
   </si>
   <si>
+    <t>Louis V Link</t>
+  </si>
+  <si>
+    <t>Some copy about Louis V</t>
+  </si>
+  <si>
     <t>MAC</t>
+  </si>
+  <si>
+    <t>MAC Link</t>
+  </si>
+  <si>
+    <t>Some copy about MAC</t>
+  </si>
+  <si>
+    <t>Calvin Klein</t>
+  </si>
+  <si>
+    <t>Calvin Klein Link</t>
+  </si>
+  <si>
+    <t>Some copy about Calvin Klein</t>
+  </si>
+  <si>
+    <t>Gucci</t>
+  </si>
+  <si>
+    <t>Gucci Link</t>
+  </si>
+  <si>
+    <t>Some copy about Gucci</t>
   </si>
 </sst>
 </file>
@@ -1292,7 +1334,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
+    <row r="3" ht="32.25" customHeight="1">
       <c r="A3" t="s" s="5">
         <v>4</v>
       </c>
@@ -1307,79 +1349,91 @@
       <c r="F3" s="6"/>
       <c r="G3" s="6"/>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
+    <row r="4" ht="32.05" customHeight="1">
       <c r="A4" t="s" s="7">
         <v>7</v>
       </c>
       <c r="B4" t="s" s="7">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s" s="7">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="8"/>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
+    <row r="5" ht="32.05" customHeight="1">
       <c r="A5" t="s" s="7">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s" s="7">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s" s="7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
       <c r="F5" s="8"/>
       <c r="G5" s="8"/>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
+    <row r="6" ht="32.05" customHeight="1">
       <c r="A6" t="s" s="7">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s" s="7">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s" s="7">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
+    <row r="7" ht="32.05" customHeight="1">
       <c r="A7" t="s" s="7">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="7">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s" s="7">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="8"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
+    <row r="8" ht="32.05" customHeight="1">
+      <c r="A8" t="s" s="7">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s" s="7">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s" s="7">
+        <v>21</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
     </row>
-    <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="8"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
+    <row r="9" ht="32.05" customHeight="1">
+      <c r="A9" t="s" s="7">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s" s="7">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s" s="7">
+        <v>24</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>

</xml_diff>